<commit_message>
v0.98 reagent sample file
</commit_message>
<xml_diff>
--- a/src/template/reagent_import_format.xlsx
+++ b/src/template/reagent_import_format.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hunkilim/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hunkilim/Works/Projects/ReactJs/pms/client/src/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854BC42B-6685-3D49-B530-2B5E7D0E8E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92EBD3F-AEF2-7F42-8A6B-F498C325ABCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1440" yWindow="-20520" windowWidth="30240" windowHeight="18880" xr2:uid="{B4D8988A-ADB1-384D-A93A-3B2B859ECBEE}"/>
+    <workbookView xWindow="3000" yWindow="-19820" windowWidth="30240" windowHeight="18880" xr2:uid="{B4D8988A-ADB1-384D-A93A-3B2B859ECBEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Reagent" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>ThermoFisher</t>
   </si>
@@ -46,115 +46,24 @@
     <t>Nuclease-free water</t>
   </si>
   <si>
-    <t>1 M Hepes, pH 7.5</t>
-  </si>
-  <si>
-    <t>AM9261</t>
-  </si>
-  <si>
-    <t>500 mM EDTA</t>
-  </si>
-  <si>
-    <t>AM2696</t>
-  </si>
-  <si>
-    <t>SUPERase IN*</t>
-  </si>
-  <si>
-    <t>RNase OUT*</t>
-  </si>
-  <si>
-    <t>DPBS</t>
-  </si>
-  <si>
     <t>Sigma</t>
   </si>
   <si>
-    <t>A9576-50ML</t>
-  </si>
-  <si>
-    <t>30% BSA in DPBS</t>
-  </si>
-  <si>
-    <t>18896-50ML</t>
-  </si>
-  <si>
-    <t>IGEPAL CA-630</t>
-  </si>
-  <si>
-    <t>D141-100MG</t>
-  </si>
-  <si>
-    <t>Digitonin</t>
-  </si>
-  <si>
-    <t>P8340</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100X Protease Inhibitors </t>
-  </si>
-  <si>
     <t>85558-5g</t>
   </si>
   <si>
-    <t>Spermidine</t>
-  </si>
-  <si>
     <t>63069-100ML</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"> 1M MgCl</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
     <t>T3038-1L</t>
   </si>
   <si>
-    <t>Tris-HCL</t>
-  </si>
-  <si>
-    <t>BT-21</t>
-  </si>
-  <si>
-    <t>4 M NaCl</t>
-  </si>
-  <si>
-    <t>epigenome techonologies</t>
-  </si>
-  <si>
-    <t>INTRT1014</t>
-  </si>
-  <si>
-    <t>SLCL8813</t>
-  </si>
-  <si>
-    <t>MKCN5898</t>
-  </si>
-  <si>
     <t>SLCG9138</t>
   </si>
   <si>
     <t>BCCD4296</t>
   </si>
   <si>
-    <t>BCCF1869</t>
-  </si>
-  <si>
-    <t>0000189173</t>
-  </si>
-  <si>
     <t>BCCG4247</t>
   </si>
   <si>
@@ -177,6 +86,39 @@
   </si>
   <si>
     <t>expiration</t>
+  </si>
+  <si>
+    <t>description1</t>
+  </si>
+  <si>
+    <t>description2</t>
+  </si>
+  <si>
+    <t>description3</t>
+  </si>
+  <si>
+    <t>description4</t>
+  </si>
+  <si>
+    <t>pp12345</t>
+  </si>
+  <si>
+    <t>pp12346</t>
+  </si>
+  <si>
+    <t>pp12347</t>
+  </si>
+  <si>
+    <t>pp12348</t>
+  </si>
+  <si>
+    <t>reagent2</t>
+  </si>
+  <si>
+    <t>reagent3</t>
+  </si>
+  <si>
+    <t>reagent4</t>
   </si>
 </sst>
 </file>
@@ -207,17 +149,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -266,10 +206,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CD1023-F9A4-984A-8DEC-D58284341654}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,25 +540,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>40</v>
+        <v>13</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>36</v>
+        <v>11</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -630,25 +568,43 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
       <c r="D2" s="7">
         <v>2210539</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="F2" s="9">
+        <v>45291</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <v>15630106</v>
-      </c>
-      <c r="D3" s="7">
-        <v>2337395</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>0</v>
+      <c r="F3" s="9">
+        <v>45292</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -656,170 +612,49 @@
         <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="9">
+        <v>45293</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1024974</v>
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="7">
-        <v>2734288</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
-        <v>10777019</v>
-      </c>
-      <c r="D7" s="7">
-        <v>2556412</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
-        <v>14190144</v>
-      </c>
-      <c r="D8" s="7">
-        <v>2561361</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>45294</v>
+      </c>
+      <c r="G5" t="s">
         <v>20</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>